<commit_message>
119 entries in vector, need to run logistic regression
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -2941,8 +2941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W287"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F98" workbookViewId="0">
-      <selection activeCell="K113" sqref="K113"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287:XFD287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14965,232 +14965,233 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" r:id="rId1"/>
-    <hyperlink ref="O2" r:id="rId2"/>
-    <hyperlink ref="O3" r:id="rId3"/>
-    <hyperlink ref="O4" r:id="rId4"/>
-    <hyperlink ref="O5" r:id="rId5"/>
-    <hyperlink ref="O6" r:id="rId6"/>
-    <hyperlink ref="O7" r:id="rId7"/>
-    <hyperlink ref="O8" r:id="rId8"/>
-    <hyperlink ref="O9" r:id="rId9"/>
-    <hyperlink ref="O10" r:id="rId10"/>
-    <hyperlink ref="O11" r:id="rId11"/>
-    <hyperlink ref="O12" r:id="rId12"/>
-    <hyperlink ref="O13" r:id="rId13"/>
-    <hyperlink ref="O14" r:id="rId14"/>
-    <hyperlink ref="O15" r:id="rId15"/>
-    <hyperlink ref="O16" r:id="rId16"/>
-    <hyperlink ref="O17" r:id="rId17"/>
-    <hyperlink ref="O18" r:id="rId18"/>
-    <hyperlink ref="O19" r:id="rId19"/>
-    <hyperlink ref="O20" r:id="rId20"/>
-    <hyperlink ref="O21" r:id="rId21"/>
-    <hyperlink ref="O22" r:id="rId22"/>
-    <hyperlink ref="O23" r:id="rId23"/>
-    <hyperlink ref="O24" r:id="rId24"/>
-    <hyperlink ref="O25" r:id="rId25"/>
-    <hyperlink ref="O26" r:id="rId26"/>
-    <hyperlink ref="O27" r:id="rId27"/>
-    <hyperlink ref="O28" r:id="rId28"/>
-    <hyperlink ref="O29" r:id="rId29"/>
-    <hyperlink ref="O30" r:id="rId30"/>
-    <hyperlink ref="O31" r:id="rId31"/>
-    <hyperlink ref="O32" r:id="rId32"/>
-    <hyperlink ref="O33" r:id="rId33"/>
-    <hyperlink ref="O34" r:id="rId34"/>
-    <hyperlink ref="O35" r:id="rId35"/>
-    <hyperlink ref="O36" r:id="rId36"/>
-    <hyperlink ref="O37" r:id="rId37"/>
-    <hyperlink ref="O38" r:id="rId38"/>
-    <hyperlink ref="O39" r:id="rId39"/>
-    <hyperlink ref="O40" r:id="rId40"/>
-    <hyperlink ref="O41" r:id="rId41"/>
-    <hyperlink ref="O42" r:id="rId42"/>
-    <hyperlink ref="O43" r:id="rId43"/>
-    <hyperlink ref="O44" r:id="rId44"/>
-    <hyperlink ref="O45" r:id="rId45"/>
-    <hyperlink ref="O46" r:id="rId46"/>
-    <hyperlink ref="O47" r:id="rId47"/>
-    <hyperlink ref="O48" r:id="rId48"/>
-    <hyperlink ref="O49" r:id="rId49"/>
-    <hyperlink ref="O50" r:id="rId50"/>
-    <hyperlink ref="O51" r:id="rId51"/>
-    <hyperlink ref="O52" r:id="rId52"/>
-    <hyperlink ref="O53" r:id="rId53"/>
-    <hyperlink ref="O54" r:id="rId54"/>
-    <hyperlink ref="O55" r:id="rId55"/>
-    <hyperlink ref="O56" r:id="rId56"/>
-    <hyperlink ref="O57" r:id="rId57"/>
-    <hyperlink ref="O58" r:id="rId58"/>
-    <hyperlink ref="O59" r:id="rId59"/>
-    <hyperlink ref="O60" r:id="rId60"/>
-    <hyperlink ref="O61" r:id="rId61"/>
-    <hyperlink ref="O62" r:id="rId62"/>
-    <hyperlink ref="O63" r:id="rId63"/>
-    <hyperlink ref="O64" r:id="rId64"/>
-    <hyperlink ref="O65" r:id="rId65"/>
-    <hyperlink ref="O66" r:id="rId66"/>
-    <hyperlink ref="O67" r:id="rId67"/>
-    <hyperlink ref="O68" r:id="rId68"/>
-    <hyperlink ref="O69" r:id="rId69"/>
-    <hyperlink ref="O70" r:id="rId70"/>
-    <hyperlink ref="O71" r:id="rId71"/>
-    <hyperlink ref="O72" r:id="rId72"/>
-    <hyperlink ref="O73" r:id="rId73"/>
-    <hyperlink ref="O74" r:id="rId74"/>
-    <hyperlink ref="O75" r:id="rId75"/>
-    <hyperlink ref="O76" r:id="rId76"/>
-    <hyperlink ref="O77" r:id="rId77"/>
-    <hyperlink ref="O78" r:id="rId78"/>
-    <hyperlink ref="O79" r:id="rId79"/>
-    <hyperlink ref="O80" r:id="rId80"/>
-    <hyperlink ref="O81" r:id="rId81"/>
-    <hyperlink ref="O82" r:id="rId82"/>
-    <hyperlink ref="O83" r:id="rId83"/>
-    <hyperlink ref="O84" r:id="rId84"/>
-    <hyperlink ref="O85" r:id="rId85"/>
-    <hyperlink ref="O86" r:id="rId86"/>
-    <hyperlink ref="O87" r:id="rId87"/>
-    <hyperlink ref="O88" r:id="rId88"/>
-    <hyperlink ref="O89" r:id="rId89"/>
-    <hyperlink ref="O90" r:id="rId90"/>
-    <hyperlink ref="O91" r:id="rId91"/>
-    <hyperlink ref="O92" r:id="rId92"/>
-    <hyperlink ref="O93" r:id="rId93"/>
-    <hyperlink ref="O94" r:id="rId94"/>
-    <hyperlink ref="O95" r:id="rId95"/>
-    <hyperlink ref="O96" r:id="rId96"/>
-    <hyperlink ref="O97" r:id="rId97"/>
-    <hyperlink ref="O98" r:id="rId98"/>
-    <hyperlink ref="O99" r:id="rId99"/>
-    <hyperlink ref="O100" r:id="rId100"/>
-    <hyperlink ref="O101" r:id="rId101"/>
-    <hyperlink ref="O102" r:id="rId102"/>
-    <hyperlink ref="O103" r:id="rId103"/>
-    <hyperlink ref="O104" r:id="rId104"/>
-    <hyperlink ref="O105" r:id="rId105"/>
-    <hyperlink ref="O106" r:id="rId106"/>
-    <hyperlink ref="O107" r:id="rId107"/>
-    <hyperlink ref="O108" r:id="rId108"/>
-    <hyperlink ref="O109" r:id="rId109"/>
-    <hyperlink ref="O110" r:id="rId110"/>
-    <hyperlink ref="O111" r:id="rId111"/>
-    <hyperlink ref="O112" r:id="rId112"/>
+    <hyperlink ref="O286" r:id="rId1"/>
+    <hyperlink ref="O284" r:id="rId2"/>
+    <hyperlink ref="O283" r:id="rId3"/>
+    <hyperlink ref="O280" r:id="rId4"/>
+    <hyperlink ref="O278" r:id="rId5"/>
+    <hyperlink ref="O277" r:id="rId6"/>
+    <hyperlink ref="O275" r:id="rId7"/>
+    <hyperlink ref="O268" r:id="rId8"/>
+    <hyperlink ref="O267" r:id="rId9"/>
+    <hyperlink ref="O266" r:id="rId10"/>
+    <hyperlink ref="O263" r:id="rId11"/>
+    <hyperlink ref="O261" r:id="rId12"/>
+    <hyperlink ref="O259" r:id="rId13"/>
+    <hyperlink ref="O252" r:id="rId14"/>
+    <hyperlink ref="O228" r:id="rId15"/>
+    <hyperlink ref="O222" r:id="rId16"/>
+    <hyperlink ref="O221" r:id="rId17"/>
+    <hyperlink ref="O220" r:id="rId18"/>
+    <hyperlink ref="O219" r:id="rId19"/>
+    <hyperlink ref="O218" r:id="rId20"/>
+    <hyperlink ref="O216" r:id="rId21"/>
+    <hyperlink ref="O215" r:id="rId22"/>
+    <hyperlink ref="O214" r:id="rId23"/>
+    <hyperlink ref="O212" r:id="rId24"/>
+    <hyperlink ref="O211" r:id="rId25"/>
+    <hyperlink ref="O210" r:id="rId26"/>
+    <hyperlink ref="O209" r:id="rId27"/>
+    <hyperlink ref="O208" r:id="rId28"/>
+    <hyperlink ref="O207" r:id="rId29"/>
+    <hyperlink ref="O206" r:id="rId30"/>
+    <hyperlink ref="O205" r:id="rId31"/>
+    <hyperlink ref="O204" r:id="rId32"/>
+    <hyperlink ref="O203" r:id="rId33"/>
+    <hyperlink ref="O202" r:id="rId34"/>
+    <hyperlink ref="O201" r:id="rId35"/>
+    <hyperlink ref="O200" r:id="rId36"/>
+    <hyperlink ref="O199" r:id="rId37"/>
+    <hyperlink ref="O198" r:id="rId38"/>
+    <hyperlink ref="O197" r:id="rId39"/>
+    <hyperlink ref="O195" r:id="rId40"/>
+    <hyperlink ref="O190" r:id="rId41"/>
+    <hyperlink ref="O189" r:id="rId42"/>
+    <hyperlink ref="O188" r:id="rId43"/>
+    <hyperlink ref="O187" r:id="rId44"/>
+    <hyperlink ref="O185" r:id="rId45"/>
+    <hyperlink ref="O184" r:id="rId46"/>
+    <hyperlink ref="O183" r:id="rId47"/>
+    <hyperlink ref="O182" r:id="rId48"/>
+    <hyperlink ref="O180" r:id="rId49"/>
+    <hyperlink ref="O179" r:id="rId50"/>
+    <hyperlink ref="O178" r:id="rId51"/>
+    <hyperlink ref="O177" r:id="rId52"/>
+    <hyperlink ref="O174" r:id="rId53"/>
+    <hyperlink ref="O173" r:id="rId54"/>
+    <hyperlink ref="O172" r:id="rId55"/>
+    <hyperlink ref="O171" r:id="rId56"/>
+    <hyperlink ref="O170" r:id="rId57"/>
+    <hyperlink ref="O169" r:id="rId58"/>
+    <hyperlink ref="O168" r:id="rId59"/>
+    <hyperlink ref="O167" r:id="rId60"/>
+    <hyperlink ref="O166" r:id="rId61"/>
+    <hyperlink ref="O165" r:id="rId62"/>
+    <hyperlink ref="O164" r:id="rId63"/>
+    <hyperlink ref="O163" r:id="rId64"/>
+    <hyperlink ref="O162" r:id="rId65"/>
+    <hyperlink ref="O161" r:id="rId66"/>
+    <hyperlink ref="O160" r:id="rId67"/>
+    <hyperlink ref="O159" r:id="rId68"/>
+    <hyperlink ref="O158" r:id="rId69"/>
+    <hyperlink ref="O157" r:id="rId70"/>
+    <hyperlink ref="O156" r:id="rId71"/>
+    <hyperlink ref="O155" r:id="rId72"/>
+    <hyperlink ref="O154" r:id="rId73"/>
+    <hyperlink ref="O153" r:id="rId74"/>
+    <hyperlink ref="O152" r:id="rId75"/>
+    <hyperlink ref="O151" r:id="rId76"/>
+    <hyperlink ref="O150" r:id="rId77"/>
+    <hyperlink ref="O149" r:id="rId78"/>
+    <hyperlink ref="O148" r:id="rId79"/>
+    <hyperlink ref="O147" r:id="rId80"/>
+    <hyperlink ref="O146" r:id="rId81"/>
+    <hyperlink ref="O145" r:id="rId82"/>
+    <hyperlink ref="O144" r:id="rId83"/>
+    <hyperlink ref="O143" r:id="rId84"/>
+    <hyperlink ref="O142" r:id="rId85"/>
+    <hyperlink ref="O141" r:id="rId86"/>
+    <hyperlink ref="O140" r:id="rId87"/>
+    <hyperlink ref="O139" r:id="rId88"/>
+    <hyperlink ref="O138" r:id="rId89"/>
+    <hyperlink ref="O137" r:id="rId90"/>
+    <hyperlink ref="O136" r:id="rId91"/>
+    <hyperlink ref="O135" r:id="rId92"/>
+    <hyperlink ref="O134" r:id="rId93"/>
+    <hyperlink ref="O133" r:id="rId94"/>
+    <hyperlink ref="O132" r:id="rId95"/>
+    <hyperlink ref="O131" r:id="rId96"/>
+    <hyperlink ref="O130" r:id="rId97"/>
+    <hyperlink ref="O129" r:id="rId98"/>
+    <hyperlink ref="O128" r:id="rId99"/>
+    <hyperlink ref="O127" r:id="rId100"/>
+    <hyperlink ref="O126" r:id="rId101"/>
+    <hyperlink ref="O125" r:id="rId102"/>
+    <hyperlink ref="O124" r:id="rId103"/>
+    <hyperlink ref="O123" r:id="rId104"/>
+    <hyperlink ref="O122" r:id="rId105"/>
+    <hyperlink ref="O121" r:id="rId106"/>
+    <hyperlink ref="O120" r:id="rId107"/>
+    <hyperlink ref="O119" r:id="rId108"/>
+    <hyperlink ref="O118" r:id="rId109"/>
+    <hyperlink ref="O117" r:id="rId110"/>
+    <hyperlink ref="O116" r:id="rId111"/>
+    <hyperlink ref="O115" r:id="rId112"/>
     <hyperlink ref="O114" r:id="rId113"/>
-    <hyperlink ref="O115" r:id="rId114"/>
-    <hyperlink ref="O116" r:id="rId115"/>
-    <hyperlink ref="O117" r:id="rId116"/>
-    <hyperlink ref="O118" r:id="rId117"/>
-    <hyperlink ref="O119" r:id="rId118"/>
-    <hyperlink ref="O120" r:id="rId119"/>
-    <hyperlink ref="O121" r:id="rId120"/>
-    <hyperlink ref="O122" r:id="rId121"/>
-    <hyperlink ref="O123" r:id="rId122"/>
-    <hyperlink ref="O124" r:id="rId123"/>
-    <hyperlink ref="O125" r:id="rId124"/>
-    <hyperlink ref="O126" r:id="rId125"/>
-    <hyperlink ref="O127" r:id="rId126"/>
-    <hyperlink ref="O128" r:id="rId127"/>
-    <hyperlink ref="O129" r:id="rId128"/>
-    <hyperlink ref="O130" r:id="rId129"/>
-    <hyperlink ref="O131" r:id="rId130"/>
-    <hyperlink ref="O132" r:id="rId131"/>
-    <hyperlink ref="O133" r:id="rId132"/>
-    <hyperlink ref="O134" r:id="rId133"/>
-    <hyperlink ref="O135" r:id="rId134"/>
-    <hyperlink ref="O136" r:id="rId135"/>
-    <hyperlink ref="O137" r:id="rId136"/>
-    <hyperlink ref="O138" r:id="rId137"/>
-    <hyperlink ref="O139" r:id="rId138"/>
-    <hyperlink ref="O140" r:id="rId139"/>
-    <hyperlink ref="O141" r:id="rId140"/>
-    <hyperlink ref="O142" r:id="rId141"/>
-    <hyperlink ref="O143" r:id="rId142"/>
-    <hyperlink ref="O144" r:id="rId143"/>
-    <hyperlink ref="O145" r:id="rId144"/>
-    <hyperlink ref="O146" r:id="rId145"/>
-    <hyperlink ref="O147" r:id="rId146"/>
-    <hyperlink ref="O148" r:id="rId147"/>
-    <hyperlink ref="O149" r:id="rId148"/>
-    <hyperlink ref="O150" r:id="rId149"/>
-    <hyperlink ref="O151" r:id="rId150"/>
-    <hyperlink ref="O152" r:id="rId151"/>
-    <hyperlink ref="O153" r:id="rId152"/>
-    <hyperlink ref="O154" r:id="rId153"/>
-    <hyperlink ref="O155" r:id="rId154"/>
-    <hyperlink ref="O156" r:id="rId155"/>
-    <hyperlink ref="O157" r:id="rId156"/>
-    <hyperlink ref="O158" r:id="rId157"/>
-    <hyperlink ref="O159" r:id="rId158"/>
-    <hyperlink ref="O160" r:id="rId159"/>
-    <hyperlink ref="O161" r:id="rId160"/>
-    <hyperlink ref="O162" r:id="rId161"/>
-    <hyperlink ref="O163" r:id="rId162"/>
-    <hyperlink ref="O164" r:id="rId163"/>
-    <hyperlink ref="O165" r:id="rId164"/>
-    <hyperlink ref="O166" r:id="rId165"/>
-    <hyperlink ref="O167" r:id="rId166"/>
-    <hyperlink ref="O168" r:id="rId167"/>
-    <hyperlink ref="O169" r:id="rId168"/>
-    <hyperlink ref="O170" r:id="rId169"/>
-    <hyperlink ref="O171" r:id="rId170"/>
-    <hyperlink ref="O172" r:id="rId171"/>
-    <hyperlink ref="O173" r:id="rId172"/>
-    <hyperlink ref="O174" r:id="rId173"/>
-    <hyperlink ref="O177" r:id="rId174"/>
-    <hyperlink ref="O178" r:id="rId175"/>
-    <hyperlink ref="O179" r:id="rId176"/>
-    <hyperlink ref="O180" r:id="rId177"/>
-    <hyperlink ref="O182" r:id="rId178"/>
-    <hyperlink ref="O183" r:id="rId179"/>
-    <hyperlink ref="O184" r:id="rId180"/>
-    <hyperlink ref="O185" r:id="rId181"/>
-    <hyperlink ref="O187" r:id="rId182"/>
-    <hyperlink ref="O188" r:id="rId183"/>
-    <hyperlink ref="O189" r:id="rId184"/>
-    <hyperlink ref="O190" r:id="rId185"/>
-    <hyperlink ref="O195" r:id="rId186"/>
-    <hyperlink ref="O197" r:id="rId187"/>
-    <hyperlink ref="O198" r:id="rId188"/>
-    <hyperlink ref="O199" r:id="rId189"/>
-    <hyperlink ref="O200" r:id="rId190"/>
-    <hyperlink ref="O201" r:id="rId191"/>
-    <hyperlink ref="O202" r:id="rId192"/>
-    <hyperlink ref="O203" r:id="rId193"/>
-    <hyperlink ref="O204" r:id="rId194"/>
-    <hyperlink ref="O205" r:id="rId195"/>
-    <hyperlink ref="O206" r:id="rId196"/>
-    <hyperlink ref="O207" r:id="rId197"/>
-    <hyperlink ref="O208" r:id="rId198"/>
-    <hyperlink ref="O209" r:id="rId199"/>
-    <hyperlink ref="O210" r:id="rId200"/>
-    <hyperlink ref="O211" r:id="rId201"/>
-    <hyperlink ref="O212" r:id="rId202"/>
-    <hyperlink ref="O214" r:id="rId203"/>
-    <hyperlink ref="O215" r:id="rId204"/>
-    <hyperlink ref="O216" r:id="rId205"/>
-    <hyperlink ref="O218" r:id="rId206"/>
-    <hyperlink ref="O219" r:id="rId207"/>
-    <hyperlink ref="O220" r:id="rId208"/>
-    <hyperlink ref="O221" r:id="rId209"/>
-    <hyperlink ref="O222" r:id="rId210"/>
-    <hyperlink ref="O228" r:id="rId211"/>
-    <hyperlink ref="O252" r:id="rId212"/>
-    <hyperlink ref="O259" r:id="rId213"/>
-    <hyperlink ref="O261" r:id="rId214"/>
-    <hyperlink ref="O263" r:id="rId215"/>
-    <hyperlink ref="O266" r:id="rId216"/>
-    <hyperlink ref="O267" r:id="rId217"/>
-    <hyperlink ref="O268" r:id="rId218"/>
-    <hyperlink ref="O275" r:id="rId219"/>
-    <hyperlink ref="O277" r:id="rId220"/>
-    <hyperlink ref="O278" r:id="rId221"/>
-    <hyperlink ref="O280" r:id="rId222"/>
-    <hyperlink ref="O283" r:id="rId223"/>
-    <hyperlink ref="O284" r:id="rId224"/>
-    <hyperlink ref="O286" r:id="rId225"/>
+    <hyperlink ref="O112" r:id="rId114"/>
+    <hyperlink ref="O111" r:id="rId115"/>
+    <hyperlink ref="O110" r:id="rId116"/>
+    <hyperlink ref="O109" r:id="rId117"/>
+    <hyperlink ref="O108" r:id="rId118"/>
+    <hyperlink ref="O107" r:id="rId119"/>
+    <hyperlink ref="O106" r:id="rId120"/>
+    <hyperlink ref="O105" r:id="rId121"/>
+    <hyperlink ref="O104" r:id="rId122"/>
+    <hyperlink ref="O103" r:id="rId123"/>
+    <hyperlink ref="O102" r:id="rId124"/>
+    <hyperlink ref="O101" r:id="rId125"/>
+    <hyperlink ref="O100" r:id="rId126"/>
+    <hyperlink ref="O99" r:id="rId127"/>
+    <hyperlink ref="O98" r:id="rId128"/>
+    <hyperlink ref="O97" r:id="rId129"/>
+    <hyperlink ref="O96" r:id="rId130"/>
+    <hyperlink ref="O95" r:id="rId131"/>
+    <hyperlink ref="O94" r:id="rId132"/>
+    <hyperlink ref="O93" r:id="rId133"/>
+    <hyperlink ref="O92" r:id="rId134"/>
+    <hyperlink ref="O91" r:id="rId135"/>
+    <hyperlink ref="O90" r:id="rId136"/>
+    <hyperlink ref="O89" r:id="rId137"/>
+    <hyperlink ref="O88" r:id="rId138"/>
+    <hyperlink ref="O87" r:id="rId139"/>
+    <hyperlink ref="O86" r:id="rId140"/>
+    <hyperlink ref="O85" r:id="rId141"/>
+    <hyperlink ref="O84" r:id="rId142"/>
+    <hyperlink ref="O83" r:id="rId143"/>
+    <hyperlink ref="O82" r:id="rId144"/>
+    <hyperlink ref="O81" r:id="rId145"/>
+    <hyperlink ref="O80" r:id="rId146"/>
+    <hyperlink ref="O79" r:id="rId147"/>
+    <hyperlink ref="O78" r:id="rId148"/>
+    <hyperlink ref="O77" r:id="rId149"/>
+    <hyperlink ref="O76" r:id="rId150"/>
+    <hyperlink ref="O75" r:id="rId151"/>
+    <hyperlink ref="O74" r:id="rId152"/>
+    <hyperlink ref="O73" r:id="rId153"/>
+    <hyperlink ref="O72" r:id="rId154"/>
+    <hyperlink ref="O71" r:id="rId155"/>
+    <hyperlink ref="O70" r:id="rId156"/>
+    <hyperlink ref="O69" r:id="rId157"/>
+    <hyperlink ref="O68" r:id="rId158"/>
+    <hyperlink ref="O67" r:id="rId159"/>
+    <hyperlink ref="O66" r:id="rId160"/>
+    <hyperlink ref="O65" r:id="rId161"/>
+    <hyperlink ref="O64" r:id="rId162"/>
+    <hyperlink ref="O63" r:id="rId163"/>
+    <hyperlink ref="O62" r:id="rId164"/>
+    <hyperlink ref="O61" r:id="rId165"/>
+    <hyperlink ref="O60" r:id="rId166"/>
+    <hyperlink ref="O59" r:id="rId167"/>
+    <hyperlink ref="O58" r:id="rId168"/>
+    <hyperlink ref="O57" r:id="rId169"/>
+    <hyperlink ref="O56" r:id="rId170"/>
+    <hyperlink ref="O55" r:id="rId171"/>
+    <hyperlink ref="O54" r:id="rId172"/>
+    <hyperlink ref="O53" r:id="rId173"/>
+    <hyperlink ref="O52" r:id="rId174"/>
+    <hyperlink ref="O51" r:id="rId175"/>
+    <hyperlink ref="O50" r:id="rId176"/>
+    <hyperlink ref="O49" r:id="rId177"/>
+    <hyperlink ref="O48" r:id="rId178"/>
+    <hyperlink ref="O47" r:id="rId179"/>
+    <hyperlink ref="O46" r:id="rId180"/>
+    <hyperlink ref="O45" r:id="rId181"/>
+    <hyperlink ref="O44" r:id="rId182"/>
+    <hyperlink ref="O43" r:id="rId183"/>
+    <hyperlink ref="O42" r:id="rId184"/>
+    <hyperlink ref="O41" r:id="rId185"/>
+    <hyperlink ref="O40" r:id="rId186"/>
+    <hyperlink ref="O39" r:id="rId187"/>
+    <hyperlink ref="O38" r:id="rId188"/>
+    <hyperlink ref="O37" r:id="rId189"/>
+    <hyperlink ref="O36" r:id="rId190"/>
+    <hyperlink ref="O35" r:id="rId191"/>
+    <hyperlink ref="O34" r:id="rId192"/>
+    <hyperlink ref="O33" r:id="rId193"/>
+    <hyperlink ref="O32" r:id="rId194"/>
+    <hyperlink ref="O31" r:id="rId195"/>
+    <hyperlink ref="O30" r:id="rId196"/>
+    <hyperlink ref="O29" r:id="rId197"/>
+    <hyperlink ref="O28" r:id="rId198"/>
+    <hyperlink ref="O27" r:id="rId199"/>
+    <hyperlink ref="O26" r:id="rId200"/>
+    <hyperlink ref="O25" r:id="rId201"/>
+    <hyperlink ref="O24" r:id="rId202"/>
+    <hyperlink ref="O23" r:id="rId203"/>
+    <hyperlink ref="O22" r:id="rId204"/>
+    <hyperlink ref="O21" r:id="rId205"/>
+    <hyperlink ref="O20" r:id="rId206"/>
+    <hyperlink ref="O19" r:id="rId207"/>
+    <hyperlink ref="O18" r:id="rId208"/>
+    <hyperlink ref="O17" r:id="rId209"/>
+    <hyperlink ref="O16" r:id="rId210"/>
+    <hyperlink ref="O15" r:id="rId211"/>
+    <hyperlink ref="O14" r:id="rId212"/>
+    <hyperlink ref="O13" r:id="rId213"/>
+    <hyperlink ref="O12" r:id="rId214"/>
+    <hyperlink ref="O11" r:id="rId215"/>
+    <hyperlink ref="O10" r:id="rId216"/>
+    <hyperlink ref="O9" r:id="rId217"/>
+    <hyperlink ref="O8" r:id="rId218"/>
+    <hyperlink ref="O7" r:id="rId219"/>
+    <hyperlink ref="O6" r:id="rId220"/>
+    <hyperlink ref="O5" r:id="rId221"/>
+    <hyperlink ref="O4" r:id="rId222"/>
+    <hyperlink ref="O3" r:id="rId223"/>
+    <hyperlink ref="O2" r:id="rId224"/>
+    <hyperlink ref="O1" r:id="rId225"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>